<commit_message>
add 5 to 9 mnist fashion quanv results
</commit_message>
<xml_diff>
--- a/check.xlsx
+++ b/check.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\haime\OneDrive\Documents\GitHub\GeneticCircuit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8A37449-BDEF-4A95-9D3A-4A69A575D511}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11DB32A9-70A1-473A-8583-FE2F0EC909B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -76,7 +76,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -107,12 +107,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -126,15 +120,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -419,7 +411,7 @@
   <dimension ref="A2:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -449,7 +441,7 @@
       <c r="B3">
         <v>2</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="6">
         <v>2</v>
       </c>
       <c r="F3">
@@ -466,7 +458,7 @@
       <c r="B4">
         <v>2</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="6">
         <v>2</v>
       </c>
       <c r="F4">
@@ -483,7 +475,7 @@
       <c r="B5">
         <v>2</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="6">
         <v>2</v>
       </c>
       <c r="F5">
@@ -500,7 +492,7 @@
       <c r="B6">
         <v>2</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="6">
         <v>2</v>
       </c>
     </row>
@@ -511,8 +503,8 @@
       <c r="B7">
         <v>2</v>
       </c>
-      <c r="C7" s="5">
-        <v>1</v>
+      <c r="C7" s="6">
+        <v>2</v>
       </c>
       <c r="F7" t="s">
         <v>7</v>
@@ -525,8 +517,8 @@
       <c r="B8">
         <v>2</v>
       </c>
-      <c r="C8" s="5">
-        <v>1</v>
+      <c r="C8" s="6">
+        <v>2</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>8</v>
@@ -539,8 +531,8 @@
       <c r="B9">
         <v>2</v>
       </c>
-      <c r="C9" s="5">
-        <v>1</v>
+      <c r="C9" s="6">
+        <v>2</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>9</v>
@@ -553,8 +545,8 @@
       <c r="B10">
         <v>2</v>
       </c>
-      <c r="C10" s="7">
-        <v>1</v>
+      <c r="C10" s="6">
+        <v>2</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>10</v>
@@ -567,8 +559,8 @@
       <c r="B11" s="1">
         <v>1</v>
       </c>
-      <c r="C11" s="7">
-        <v>1</v>
+      <c r="C11" s="6">
+        <v>2</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>11</v>
@@ -581,8 +573,8 @@
       <c r="B12" s="1">
         <v>1</v>
       </c>
-      <c r="C12" s="7">
-        <v>1</v>
+      <c r="C12" s="6">
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -622,8 +614,8 @@
       <c r="A16">
         <v>14</v>
       </c>
-      <c r="B16">
-        <v>0</v>
+      <c r="B16" s="3">
+        <v>1</v>
       </c>
       <c r="C16">
         <v>2</v>
@@ -633,8 +625,8 @@
       <c r="A17">
         <v>15</v>
       </c>
-      <c r="B17">
-        <v>0</v>
+      <c r="B17" s="3">
+        <v>1</v>
       </c>
       <c r="C17">
         <v>2</v>
@@ -647,7 +639,7 @@
       <c r="B18" s="4">
         <v>1</v>
       </c>
-      <c r="C18" s="6">
+      <c r="C18" s="5">
         <v>2</v>
       </c>
     </row>
@@ -658,7 +650,7 @@
       <c r="B19" s="4">
         <v>1</v>
       </c>
-      <c r="C19" s="6">
+      <c r="C19" s="5">
         <v>2</v>
       </c>
     </row>
@@ -669,7 +661,7 @@
       <c r="B20" s="4">
         <v>1</v>
       </c>
-      <c r="C20" s="6">
+      <c r="C20" s="5">
         <v>2</v>
       </c>
     </row>
@@ -680,7 +672,7 @@
       <c r="B21" s="4">
         <v>1</v>
       </c>
-      <c r="C21" s="6">
+      <c r="C21" s="5">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add 9 10 and 16 17 quanv mnist result
</commit_message>
<xml_diff>
--- a/check.xlsx
+++ b/check.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\haime\OneDrive\Documents\GitHub\GeneticCircuit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11DB32A9-70A1-473A-8583-FE2F0EC909B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C98ECE55-98D6-42E9-86EB-8EDD92663A7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -411,7 +411,7 @@
   <dimension ref="A2:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -556,8 +556,8 @@
       <c r="A11">
         <v>9</v>
       </c>
-      <c r="B11" s="1">
-        <v>1</v>
+      <c r="B11" s="5">
+        <v>2</v>
       </c>
       <c r="C11" s="6">
         <v>2</v>
@@ -570,8 +570,8 @@
       <c r="A12">
         <v>10</v>
       </c>
-      <c r="B12" s="1">
-        <v>1</v>
+      <c r="B12" s="5">
+        <v>2</v>
       </c>
       <c r="C12" s="6">
         <v>2</v>
@@ -636,8 +636,8 @@
       <c r="A18">
         <v>16</v>
       </c>
-      <c r="B18" s="4">
-        <v>1</v>
+      <c r="B18" s="5">
+        <v>2</v>
       </c>
       <c r="C18" s="5">
         <v>2</v>
@@ -647,8 +647,8 @@
       <c r="A19">
         <v>17</v>
       </c>
-      <c r="B19" s="4">
-        <v>1</v>
+      <c r="B19" s="5">
+        <v>2</v>
       </c>
       <c r="C19" s="5">
         <v>2</v>
@@ -658,7 +658,7 @@
       <c r="A20">
         <v>18</v>
       </c>
-      <c r="B20" s="4">
+      <c r="B20" s="2">
         <v>1</v>
       </c>
       <c r="C20" s="5">
@@ -669,7 +669,7 @@
       <c r="A21">
         <v>19</v>
       </c>
-      <c r="B21" s="4">
+      <c r="B21" s="2">
         <v>1</v>
       </c>
       <c r="C21" s="5">

</xml_diff>

<commit_message>
Update multifilter quanv layer
</commit_message>
<xml_diff>
--- a/check.xlsx
+++ b/check.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\haime\OneDrive\Documents\GitHub\GeneticCircuit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C98ECE55-98D6-42E9-86EB-8EDD92663A7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A2F7893-87D0-45FA-85A5-F55F1E0FBA9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -408,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:G21"/>
+  <dimension ref="A2:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -436,24 +436,18 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
-      <c r="C3" s="6">
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3" t="s">
-        <v>4</v>
+      <c r="C3">
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -462,15 +456,15 @@
         <v>2</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -479,40 +473,43 @@
         <v>2</v>
       </c>
       <c r="F5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6">
         <v>2</v>
       </c>
       <c r="C6" s="6">
         <v>2</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7">
         <v>2</v>
       </c>
       <c r="C7" s="6">
         <v>2</v>
-      </c>
-      <c r="F7" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8">
         <v>2</v>
@@ -520,13 +517,13 @@
       <c r="C8" s="6">
         <v>2</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>8</v>
+      <c r="F8" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9">
         <v>2</v>
@@ -534,13 +531,13 @@
       <c r="C9" s="6">
         <v>2</v>
       </c>
-      <c r="F9" s="2" t="s">
-        <v>9</v>
+      <c r="F9" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10">
         <v>2</v>
@@ -548,49 +545,52 @@
       <c r="C10" s="6">
         <v>2</v>
       </c>
-      <c r="F10" s="3" t="s">
-        <v>10</v>
+      <c r="F10" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>9</v>
-      </c>
-      <c r="B11" s="5">
+        <v>8</v>
+      </c>
+      <c r="B11">
         <v>2</v>
       </c>
       <c r="C11" s="6">
         <v>2</v>
       </c>
-      <c r="F11" s="4" t="s">
-        <v>11</v>
+      <c r="F11" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" s="5">
         <v>2</v>
       </c>
       <c r="C12" s="6">
         <v>2</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>11</v>
-      </c>
-      <c r="B13">
-        <v>2</v>
-      </c>
-      <c r="C13">
+        <v>10</v>
+      </c>
+      <c r="B13" s="5">
+        <v>2</v>
+      </c>
+      <c r="C13" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14">
         <v>2</v>
@@ -601,7 +601,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -612,10 +612,10 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>14</v>
-      </c>
-      <c r="B16" s="3">
-        <v>1</v>
+        <v>13</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
       </c>
       <c r="C16">
         <v>2</v>
@@ -623,7 +623,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17" s="3">
         <v>1</v>
@@ -634,18 +634,18 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18" s="5">
         <v>2</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18">
         <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B19" s="5">
         <v>2</v>
@@ -656,10 +656,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>18</v>
-      </c>
-      <c r="B20" s="2">
-        <v>1</v>
+        <v>17</v>
+      </c>
+      <c r="B20" s="5">
+        <v>2</v>
       </c>
       <c r="C20" s="5">
         <v>2</v>
@@ -667,12 +667,23 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B21" s="2">
         <v>1</v>
       </c>
       <c r="C21" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>19</v>
+      </c>
+      <c r="B22" s="1">
+        <v>1</v>
+      </c>
+      <c r="C22" s="5">
         <v>2</v>
       </c>
     </row>

</xml_diff>